<commit_message>
Save progress on FeatureEquivalenceCalculator.
</commit_message>
<xml_diff>
--- a/data/fit_result_tf.xlsx
+++ b/data/fit_result_tf.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">group</t>
   </si>
   <si>
-    <t xml:space="preserve">GENE_ID</t>
+    <t xml:space="preserve">feature</t>
   </si>
   <si>
     <t xml:space="preserve">score</t>
@@ -334,6 +334,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -355,6 +356,7 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -432,15 +434,15 @@
   <dimension ref="A1:E354"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.94"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>

</xml_diff>